<commit_message>
Get daily reddit data: Tue Mar 12 08:07:47 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_17.xlsx
+++ b/data/2024_03_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C463"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2760 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1bcoxbn</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Did my nails acrylic? I don't know what to paint them</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcjajddl3unc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1bcoob4</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Third time ever doing acrylic nails/ gel nails.</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnzjj2w31unc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1bco5w9</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Loving this matte nude set!</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsb83tkdwtnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1bcnzju</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>mermaid chrome nails 🧜🫧🐚</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcnzju</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1bcmkur</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>My partner is (heavily) hinting at proposing soon and I'm feeling insecure about my nails</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcmkur</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1bcmik8</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel-X burns so bad </t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bcmik8/gelx_burns_so_bad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1bclood</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>3 days of painting on small nails, worth the back pain</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tg6zobvqatnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1bcniay</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Green for st. patty’s day 🍀</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz6djg8hqtnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1bcik2p</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Nailart inspired by Nezuko Kamado (Demon Slayer Anime)</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq7rluoxlsnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1bcfy9y</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>nail fail fixed</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcfy9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1bcn0k8</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>9 days since I got my nails done</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fv3sn2q4mtnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1bcmqlr</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Colors for pale skin?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bcmqlr/colors_for_pale_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1bcmj2b</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Some recent sets</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcmj2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1bcm5n8</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>First set</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcm5n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1bcl5ya</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Did my first set of french tips</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcl5ya</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1bckgjx</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Close up shots of some nails I did last week ✨ all sets but the last are natural nails with hard gel overlays. The last set has extensions</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bckgjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1bcjiyn</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Still learning, any help appreciated</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcjiyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1bcittn</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Which do You like best? Suggestions for future sets welcome!</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcittn</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1bciqht</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Just finished my nails after spending 2 hours on them and they’re hilariously bad. I can’t stop laughing.</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bciqht</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1bchxd9</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Just got this set!</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bchxd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1bchx07</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Best option for a "one and done" service for wedding day?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bchx07/best_option_for_a_one_and_done_service_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1bchp5j</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Florals for spring! Fighting my phone to get a good picture is no fun 😔</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bchp5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1bcgti9</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bcgti9/question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1bcgsl9</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Gel-X set </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3w0dndc69snc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1bcgink</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Protecting Nails During Exercise? </t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bcgink/protecting_nails_during_exercise/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1bcghcu</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Need Advice</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcghcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1bcfccg</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>I know it’s not perfect…</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcfccg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1bcf71u</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>I love the clash of color</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3f8i8y43yrnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1bcf1xw</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>I’m in love with my nails 🥰</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88svmaz2xrnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1bcefjp</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>🍓🍫Apollo Chocolate Packaging Nails🍫🍓</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ziysf49ssrnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1bce9y7</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>March froggie nails</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w15kb3porrnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1bce5py</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>New shape and length</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bce5py</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1bcdwto</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>White with pink chrome :)</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2olo92w5prnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1bcd0ea</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling a bit like Regina George. Poly get set for March </t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b29wwg70jrnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1bcc93x</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it’s not valentines but i love red nails and cute hearts! new set ❤️😩 </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohae0ojsdrnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1bcbp3z</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>In love with this colour! What do you think?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ac4veaw9rnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1bcbiw0</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Dreamy skies ✨️</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcbiw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1bcb5wo</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>from this mornings set 💜</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhov00v76rnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1bcb5bd</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Am I Lame for Wanting to keep my nails the same all the time?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bcb5bd/am_i_lame_for_wanting_to_keep_my_nails_the_same/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1bcb4xs</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Why is this one nail glowing? I did it a week ago</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnh8t1326rnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1bcatht</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Pre Bday Nails</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcatht</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1bcaqhs</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>New nails 🔥🔥</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhkpwhr83rnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1bc9zdq</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>I called these my Elsa set ❄️</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc9zdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1bc9wd8</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polygel or Dip powder ? </t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bc9wd8/polygel_or_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1bc9r0b</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Spring nails 💐</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xe6vmf5wqnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1bc9qq3</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Did my nails last night. In love with this cherry red</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc9qq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1bc9lda</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Witchy vibes</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6hwwy14vqnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1bc93hv</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Letting my Nailtech decide the design is always the best option</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc93hv</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1bc8mf1</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>totally radical skateboarding cinamaroll nails</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc8mf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1bc8bzl</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Help please</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bc8bzl/help_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1bc7ebm</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>A new set🥰</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci3jy4qdfqnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1bc76kl</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Strengthening the nail bed</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhzzs7zvdqnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1bc74sq</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>ISO Product to support brittle weak nails (something like dip build powder)</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bc74sq/iso_product_to_support_brittle_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1bc744t</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>St. Patrick’s Day nails</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vd1ex5qedqnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1bc6yoz</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Sky bears 🌙</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avf7212ccqnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1bc6jb7</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>My 2nd set ever! ✨😄💃🏻</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc6jb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1bc5pr4</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Starting to dabble in nail art/DIY press ones, and need some advice</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bc5pr4/starting_to_dabble_in_nail_artdiy_press_ones_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1bc3reg</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why are my nails growing in angled instead of arched? </t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tid9oiinpnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1bc2m7u</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>matte non wipe vs wipe</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bc2m7u/matte_non_wipe_vs_wipe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1bc20xb</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Looking for CLEANEST builder gel or soft gel</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bc20xb/looking_for_cleanest_builder_gel_or_soft_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1bc1xc4</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Press-On Glue/Bond??</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bc1xc4/presson_gluebond/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1bc06cj</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Can someone please recommend a very good shiny clear topcoat for me to use on myself?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bc06cj/can_someone_please_recommend_a_very_good_shiny/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1bc68dz</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>some heart nails I did last month for Vday</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc68dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1bbw6cu</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Free edge of nails colour</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bbw6cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1bbrhu0</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Hema free semi cured gel strips?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bbrhu0/hema_free_semi_cured_gel_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1bbosu4</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Any techs in Tokyo?✨</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bbosu4/any_techs_in_tokyo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1bc50yx</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>the perfect shifty neutral ✨</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc50yx</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1bc4888</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>I never do them this long 🥰</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8og12vbrpnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1bc3hk6</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>My new set for March</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc3hk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1bc3ehh</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make nails look better while rehabbing them? They were breaking constantly (I think from too much nail polish) so I’m taking a break from polish but they look awful. Any tips for making them look a little better while waiting for them to grow out and get stronger? </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kmdqkrkkpnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1bc33qs</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>(Update) Mani/Pedi’s with MIL</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc33qs</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1bc2vjr</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Korean jelly nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwcxam50gpnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1bc2m4y</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>crackle is backle 😅</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp0xaagsdpnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1bc2aw0</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Used the water marbling technique for the first time, and definitely not the last</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc2aw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1bc24mh</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>good morning, red nails ♡</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mql6ftm99pnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1bc0pru</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Soft pink Nail Gel with glitters ✨️ </t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/og5vcvkeuonc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1bc02ms</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>I’ll forever be a firm believer in if imma get nails, imma get NAILS ✨</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3m6gpf1nonc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1bbzl63</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>French tips</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aras2d9ahonc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1bbzbok</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>+1 for sheer chrome pink 💖</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5a9acztsdonc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1bbyl0a</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>St. Patrick's day and Easter nails</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bbyl0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1bcqtrd</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do Satin finishes need a specific application to do their thing? </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bcqtrd/do_satin_finishes_need_a_specific_application_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1bcq8k7</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Those who only wear and / or paint their natural nails please say why.</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bcq8k7/those_who_only_wear_and_or_paint_their_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1bcoqnb</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Longest Lived Thermals??</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bcoqnb/longest_lived_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1bcn9mq</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I did something weird</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcn9mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1bcmvc3</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Mid-month manis!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcmvc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1bck0em</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Best “Chrome” Shimmer Polish?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gd8iz44cxsnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1bcl6dx</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>My mother loves milk white nails on her natural nails, is the Luna cover base 4 in Milky worth it? I don't want to spend 15 dollars on a dud when I can get a polish that has been on my wishlist for a while instead</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bcl6dx/my_mother_loves_milk_white_nails_on_her_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1bckygw</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Shamrock skittle for March!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bckygw</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1bcku8o</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Comparison between 2 polishes 💜💙</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcku8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1bckqh6</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>It’s giving…Dr. Pepper 🥤</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bckqh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1bckq6o</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Which brand’s glass file do you  rec?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bckq6o/which_brands_glass_file_do_you_rec/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1bckq48</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Which brand’s glass file do you  rec?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bckq48/which_brands_glass_file_do_you_rec/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1bck8uf</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Do these look super fake?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3l7spj8zsnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1bcix14</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Brand of polish that dries FAST!!</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bcix14/brand_of_polish_that_dries_fast/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1bcimc8</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Currently have really bad flimsy/thin nails from getting my nails done for 2 years straight,  but my wedding is this Friday and need help  </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bcimc8/currently_have_really_bad_flimsythin_nails_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1bcila8</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Dazzle dry first experience</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8xq7hi7msnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1bcigv5</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Accent dilemma</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcigv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1bcifiu</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>This polish is crazy</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcifiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1bchsxv</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>I love blues!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efji2f0fgsnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1bchn4l</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Absolutely swooning</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bchn4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1bchjm1</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>💕🌺🌸🎀🐷🦩</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bchjm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1bchioa</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Jade jelly</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o8yvody9esnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1bch2z0</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>My first ILNP order came in!</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bch2z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1bcgwqf</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>💜🦄😈👾☂️🌂</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcgwqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1bcgjgk</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Guess what nails I’m starting 👀</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgd9e4p67snc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1bcfoe0</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Zoya's Midori</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l12hbotd1snc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1bcf9ep</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>DVN Dill Weed over OPI You’re Such a Budapest and water decals</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nohf5ruiyrnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1bcf0cv</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Northern Lights Nails 🌌</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tfmg7ndrwrnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1bcegb1</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best gold flake topper? </t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bcegb1/best_gold_flake_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1bcdy1s</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Not sure if pickled or prugly...</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2ztg1feprnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1bcdtr9</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Wolfsbane HHC Encore &amp; Technopathy</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcdtr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1bcdris</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Cirque - Venetian Sky</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcdris</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1bcdinb</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Mooncat-Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lu1anepemrnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1bcda40</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Emily de Molly- It’s come to this</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wdyl5rzskrnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1bcd6fv</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>green nail season is my favorite nail season 💚</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/blgy82q2krnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1bccwls</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>ILNP Velveteen</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/scaismc8irnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1bccsfz</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Finally painted my nails after ages</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bccsfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1bccqhy</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Loved these, about to change them for St. Patrick’s Day.</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bccqhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1bcc2a5</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>New color new me</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p435u4lgcrnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1bcbuf0</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Didn’t hit the mark for me. What do you think?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcbuf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1bcbjm9</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Emeralds This Week</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcbjm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1bcb947</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Bluebird Lacquer 'Chloride the Lightening'</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l46iscau6rnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1bcb7i9</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>I topped a blue polish with Sassy Sauce LSD</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mfbq4gte6rnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1bcarxi</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>New fave: Embrace Change by Crystal Knockout</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcarxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1bcanvb</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Looking for more neons</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr6y85qp2rnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1bca6fj</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>regular top coat on gel nails?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bca6fj/regular_top_coat_on_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1bc9os9</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>🤍🍓Strawberries &amp; Cream🍓🤍</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc9os9</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1bc979t</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>i’m a sucker for a blue shimmer 🦋</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ymbknqt9sqnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1bc95ha</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Letting my Nailtech decide the design is always the best option</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc95ha</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1bc93ok</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Two coats of mademoiselle and one coat of good to go! I'm on a quest to find the perfect sheer pink.</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc93ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1bc8zym</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Lacquer - I’m a Hamster in a Wheel</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc8zym</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1bc7mff</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Trouble with "capping" the free edge (pic in comments)</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bc7mff/trouble_with_capping_the_free_edge_pic_in_comments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1bc7hl2</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Drugstore polish peels off but indie polishes don’t</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bc7hl2/drugstore_polish_peels_off_but_indie_polishes_dont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1bc7ehs</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>has anyone ever had their lacquers dry matte even though the polish it’s self isn’t supposed to be matte</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bc7ehs/has_anyone_ever_had_their_lacquers_dry_matte_even/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1bc70th</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Me and my dotting tool can't be separated 😀</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc70th</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1bc6zxo</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rogue Lacquer ‘it just makes me happy’ ft. my dog </t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kn4zf6lcqnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1bc6ykq</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press On Question </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bc6ykq/press_on_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1bc6s9w</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>The shift is unreal</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc6s9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1bbv3oc</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Canadian woes </t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bbv3oc/canadian_woes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1bc5xbm</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When the sun finally comes out </t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukl8q50q4qnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1bc5whf</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Black Swan in the sun</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc5whf</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1bc5jqa</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>St. Paddy’s Nails</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gc6nz2gr1qnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1bc51xe</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>the perfect shifty neutral ✨</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc51xe</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1bc4y8w</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Please share your tips and tricks for nail art photography!</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc4y8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1bc249k</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Spring is coming</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc249k</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1bc1cod</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Ugly nails update, one month of growth and care later.</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc1cod</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1bbzuop</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Should I file them all down?</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bbzuop</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1bbzn2w</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bbzn2w/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1bcngur</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>A MidnightSummer</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3h1jq2b3qtnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1bcng4z</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Red Oasis♥️</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z5ip26ywptnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1bcnef1</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Night sky🌃🌠🌛🌙⭐️✨🌟</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/05b1jbiiptnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1bclkws</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>I love these, so simple and cute. What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3y3kigiq9tnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1bcfgyb</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>I know it’s not perfect…</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcfgyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1bcf7vo</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>I love the way the color clash</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1tor5o8yrnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1bcbsb9</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>New set new me</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szzxcmkjarnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1bc9pjj</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Third time doing a soft gel set, added some gold lines</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc9pjj</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1bc4p3u</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I really like how the rainbow turned out 🍀🌈 </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr9987i2vpnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1bc35eo</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mis uñas </t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfgkuqghipnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1bc2m79</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Gel x I did</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc2m79</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1bc2952</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Tried water marbling for the first time! Messy, but worth it.</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bc2952</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1bbzpb7</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itzd6n9mionc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1bby363</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving the sparkles 💎❄️ </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lke4it0ynnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Mar 13 08:07:32 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_17.xlsx
+++ b/data/2024_03_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C463"/>
+  <dimension ref="A1:C604"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8304,6 +8304,2403 @@
         </is>
       </c>
     </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1bdlr4z</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Gel top coat over press on nails - help needed!</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdlr4z/gel_top_coat_over_press_on_nails_help_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1bdhg9f</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you use pressed glitter on your nails? If so, how? </t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdhg9f/can_you_use_pressed_glitter_on_your_nails_if_so/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1bdgs78</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ELI5: difference between acrylics/BIAB/gel extensions </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdgs78/eli5_difference_between_acrylicsbiabgel_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1bdfyui</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Acrylic Overlay or Builder Gel on natural nails?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdfyui/acrylic_overlay_or_builder_gel_on_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1bdbkpb</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>I think I'm having kind of a glazed donut moment? 😆</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdbkpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1bdl7xl</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0uy28wbw1oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1bdkvfu</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>I 🩵 my job!</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkvsdnc6s1oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1bdkpxb</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>New Press Ons</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdkpxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1bdkpr5</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Gel-x 1.5 month retention</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdkpr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1bdk4zj</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Help with my curved nails‼️</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdk4zj</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1bdj6jc</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>From a constant nail biter, to this!</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdj6jc</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1bdj0sa</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Progress 🤗</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdj0sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1bdic5c</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>I love art nails🤩</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdic5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1bdi73g</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Still so new to this, but I love these! Striving for a more even application at the nail base.</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdi73g</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1bdh7sm</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Delicate and simple... This shade of pink has me in love 💖</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhkfin5fr0oc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1bdh6u4</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Spring press ons!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdh6u4</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1bdgf4t</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Asking the nail salon to do French acrylics using the acrylic powder instead of painting the tip</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdgf4t/asking_the_nail_salon_to_do_french_acrylics_using/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1bdfu6l</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>My right hand. The hardest one lol</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ke29pao2g0oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1bdfdi3</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>chronic nail biter- these are my natural nails 💜</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/158foevcc0oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1bdf8et</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>I broke a nail. All I had was blue poly gel.</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kefjyuf7b0oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1bdf33g</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Team green or team blue? 🌲🥶</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdf33g</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1bdd4dk</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Froggy 🐸Nails for Spring</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jj0zmr3uznc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1bdckb5</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>How do y’all get your nails to stay on longer than a week?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdckb5/how_do_yall_get_your_nails_to_stay_on_longer_than/</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1bdbvxz</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Fruity 🍉🍓🍋</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdbvxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1bdblrf</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>First set of cats eye nails. Love them.</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdblrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1bdb8yx</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Boyfriend wanted to do my nails, I'm in love with them!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gjbsi7o4gznc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1bdalie</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>How do you wash your hair with gemstone-nails</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdalie/how_do_you_wash_your_hair_with_gemstonenails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1bdak4m</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Emotional post about finally having nails again</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdak4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1bd8ce0</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>So these were fun!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd8ce0</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1bd77km</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>When should I go back?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd77km</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1bd4krg</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Question on tip glue under acrylics and gel</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bd4krg/question_on_tip_glue_under_acrylics_and_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1bd3tae</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Inspired by Big Panda and Tiny Dragon</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd3tae</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1bdalur</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>I love long nails</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/325sr0jfbznc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1bd0jfr</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Yes or no? I did them. I’m a short nail girly right now lol. What I’m working with til they grow back. It’s a pink white color :)</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oaul3km1dxnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1bd9g4y</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>My most fierce set</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsc50kga3znc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1bd9b2q</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>silver chrome🩶</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd9b2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1bd8mer</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>First two times trying to do my own 'art'</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd8mer</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1bd8du7</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Some of the work done by my amazing nail tech 💅</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd8du7</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1bd877t</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Can you use peel off polish on builder gel?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bd877t/can_you_use_peel_off_polish_on_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1bd80ge</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My one perfect nail chipped off I hate everything </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4swzob9tync1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1bd7zhc</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Too soon for Spring nails or just right? 🌼</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd7zhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1bd6sra</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Close up on my thumb art 🌸</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi4wvxnpkync1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1bd6a0f</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">minimalist set </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1jtndmygync1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1bd68qf</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>💚 Painted Polish Slime All Yours 💛 I do love a good prugly green 😁</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd68qf</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1bd5x8g</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Atrocious, self-made manicure update: I’m in my redemption era!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd5x8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1bd5qdk</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>bday nails :))</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jsfqo93dync1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1bcpezh</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>I thought I did alright until I saw them in better light 😂</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcpezh</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1bd57r7</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Soft white + glitter</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd57r7</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1bd54wt</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time.</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75mjx9b49ync1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1bd53py</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Nail shape help!</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd53py</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1bco9wq</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Protein Shake Inspired</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bco9wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1bczl2k</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Beach day / Pisces set!.....but mistakes were made</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bczl2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1bd4eoi</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>feeling cretaceous</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd4eoi</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1bd49jg</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>My prettiest set so far! It’s giving coquette 🎀🩷✨</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd49jg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1bd3xjt</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Cookie...?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8n0mefm0ync1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1bd3vk7</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>green ombré polygel 💚</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd3vk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1bd3opf</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>#WeirdHandPoses</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75n3p1b2zxnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1bd3jxi</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Love them</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd3jxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1bd33jg</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>my birthday nails🐟🐟</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd33jg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1bd30dd</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Recs please for a blue np like this.</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bd30dd/recs_please_for_a_blue_np_like_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1bd2jqp</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Easter press ons O&amp;J</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd2jqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1bd1wld</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Best Nail Tech Certification in Ottawa, Ontario?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bd1wld/best_nail_tech_certification_in_ottawa_ontario/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1bd0gjs</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>What do you think of my lastest set ? Traditionl polish and aerographer 🥰</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpt97rtgcxnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1bcztoj</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>👾</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nf2msons7xnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1bcz506</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Current set by  NailzXshanti 🌸</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6xh4dzp2xnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1bcz419</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Builder gel lifts/falls off after a week?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bcz419/builder_gel_liftsfalls_off_after_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1bcyg4r</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>My first successful nails! What do you think? I’m really proud 😊</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcyg4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1bcyf0p</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Invader Zim nails.</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8cngc93xwnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1bcxzlc</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Nail stickers / short nails</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ieipse4qtwnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1bcxmjz</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>🍒</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjwyrq0tqwnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1bcxgsb</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>How easy is using the jelly stamp thing to do French tips?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ofgw0jgpwnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1bcx7lx</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The nails I used for the BARBIE premiere </t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eii7y189nwnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1bcwvat</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Dark Fairy Queen</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcwvat</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1bcws11</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>My favorite set I’ve done in a while!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfew6wmijwnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1bcvs1i</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Hard Gel Girly!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcvs1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1bct4ae</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Spicing basic nudes up and adding some flowers for spring😳</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqxllsbdhvnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1bcsysv</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Love a holo</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcsysv</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1bcsiht</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Advice please?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tumfbxv9vnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1bcs8id</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Loving my new Holo Taco nail polish in 50 Shades of Greige 🩶</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuxjgm7d6vnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1bdm0a1</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>I feel like a blue footed booby</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdm0a1</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1bdj6kf</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Really in love with my floral nails</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdj6kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1bdirth</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Update on Olive&amp; June Purple Puka Dupe</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ux07o61951oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1bdfzb3</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Lavender French Tips</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdfzb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1bdei6d</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about Dazzle Dry </t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bdei6d/question_about_dazzle_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1bdctg9</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>I feel like I've come so far in just a year!</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdctg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1bdbzyo</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Update to my last post asking for advice!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c54txkllznc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1bdbfb9</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Never gonna get over UP, tbh</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdbfb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1bdbbo8</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>The various looks I've seen over the last few days from Fancy Chameleon</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdbbo8</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1bdb9hu</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Winter Berries is such a fitting name 😍</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n9h84ss9gznc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1bdao61</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Pretty glowy purple!</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdao61</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1bdaez4</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>QotD 😍</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5f4iit2aznc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1bd88ec</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Can you put peel off polish on top of builder gel?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bd88ec/can_you_put_peel_off_polish_on_top_of_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1bd7v50</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Well well well, it's Fuck You Too-sday. 💔</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7o8gjpy7sync1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1bd7dbr</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Like gold coins amidst clover 🍀</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd7dbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1bd76sk</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>I took pictures!</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd76sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1bd67wv</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>💚 Painted Polish Slime All Yours 💛 I do love a good prugly green 😁</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd67wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1bd5hhd</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Keeping it green this week 💚</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ws7b8hqcbync1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1bd4d8e</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Never gonna give you up</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd4d8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1bd4202</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LynB’s Embrace The Mess </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bd4202/lynbs_embrace_the_mess/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1bd3ulf</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Mooncat To All Who Ghosted Me with Siren's Deceit</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd3ulf</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1bd3mun</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Shake Your Shamrock dupe</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hujxqlpyxnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1bd3jcb</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Quackpath</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u99q4et0yxnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1bd3eyn</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Clover gradient with Cirque🍀</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd3eyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1bd31yd</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>I feel like a magical Barnie 💜✨</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ict6kckouxnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1bd2ng4</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>quackpth</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd2ng4</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1bd2igt</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Had to chop everything after a series of unrecoverable breaks, figured I may as well start over with a literal blank slate</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd2igt</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1bd2ib6</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>They’re not the same..?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbq6rottqxnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1bd1c2q</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Clionadh Hippo (PPU 2/24) vs. Fairy Dust and EdM Directions to Whereabouts</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd1c2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1bd08ez</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>My pictures don’t do this polish justice 😍</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd08ez</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1bd028r</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>DVN - Star Smut</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bd028r</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1bczqbf</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>To say that I’m obsessed with this polish would be an understatement. 😍</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hp2908q17xnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1bcz591</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Lumen "Morpho Glow"</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcz591</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1bcy93b</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Oil soak for nails</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bcy93b/oil_soak_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1bcxiu0</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Can't stop staring</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1uecel2ypwnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1bcwyfh</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Pink surprise</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcwyfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1bcw9nf</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>lavender holo in sunlight ☺️</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f45ymbaxewnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1bcvrsx</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Toadstool</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcvrsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1bcv6id</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>First attempt biab+ gel</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/434w8f4i4wnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1bct9ye</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ironically, I mostly break and bend my nails while trying to press out my vitamins and supplements supposed to make my nails stronger </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/798na3jbjvnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1bcsi9a</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>PSA: If you layer Essie No to-do with Essie Bordeaux, you basically get the discontinued Essie Chocolate Cakes</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcsi9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1bcs9pm</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>I’m in love 💅🏼</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3ggfegr6vnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1bcs40z</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Bad chipping when capping tips?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bcs40z/bad_chipping_when_capping_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1bdlwy9</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>My press on set</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdlwy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1bdl6r2</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Famine</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4rt7mtxv1oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1bdkxwg</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Did some 3D veggie nails🍅</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdkxwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1bdk27b</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Spring Betty Boop🌼</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0rj3knqi1oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1bdgnln</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Did my first complex paint in a while 🥰</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdgnln</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1bdg0qh</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Death</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acawz0lih0oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1bdelbr</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Care Bear Nails 🌈🌥️🍀</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8oha8vu50oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1bdchvs</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Amethyst/Jade combo</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdchvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1bdc5gv</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Fruit! 🍉🍓🍋</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdc5gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1bdbmme</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Fade to grey, using gel and acrylic</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mme04ixiznc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1bd23tx</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Clouds x Vox Continental Organ</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4nq4492oxnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1bczqts</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Test sticks vs final result</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8mq54ts47xnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1bcz6tl</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Mooo</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xehypx33xnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1bcz5x0</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Spring set by NailzXshanti 🌸</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bguxez3x2xnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1bcylav</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>My first successful manicure on myself 😊</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcylav</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1bcxnpm</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished painting Rainbow Dash for my MLP set for Tiktok ☺️ 💕 more to come </t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yg7ggt13rwnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1bcwwpd</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Opinions/CC on these?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bcwwpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1bcwevt</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling a little green 💚 </t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8d8131i7gwnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1bctou8</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Nail Art</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bctou8</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Mar 14 08:08:07 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_17.xlsx
+++ b/data/2024_03_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C604"/>
+  <dimension ref="A1:C767"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10701,6 +10701,2778 @@
         </is>
       </c>
     </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1befqk8</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>I tried these press on nails today!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qq8doqp79oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1befjox</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Needed a big chop. I was craving the feeling of touching things. Am I the only one after months of long nails?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1befjox</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1bef0s6</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I tried drawing a Geisha LOL</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p65r99xiy8oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1beezx8</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>In my Frenchie era</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beezx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1bed2az</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Flames🔥🖤</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdlc8s69c8oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1bebjom</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech did it again. </t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nox8wns0y7oc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1bebigl</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech did it again. </t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uwntczxox7oc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1bebi10</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Nail tech freehanded all this for the Taylor swift concert. So good!</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbgvdkorx7oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1beb5mq</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Jud finished painting Fluttershy for the My Little Pony set for TikTok 💕</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vinh2emru7oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1be9vz3</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Heat/humidity/moisture and gel x question</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1be9vz3/heathumiditymoisture_and_gel_x_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1be9vix</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Are my Nails Tacky/Out of Style?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1be9vix/are_my_nails_tackyout_of_style/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1be93za</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Beetles Builder works better than top brands</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1be93za/beetles_builder_works_better_than_top_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1be91gq</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Nail biter that needs to look professional, overwhelmed with options</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be91gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1be629e</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Water nail decals? </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1be629e/water_nail_decals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1be9hai</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>DIY Nail Art</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dz2cwhvcg7oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1be8z5b</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>DND Ferrari red Nontoxic dupe ?</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1be8z5b/dnd_ferrari_red_nontoxic_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1be8j5q</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Got my nails done again! chameleon polish</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xrselghb87oc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1be89mb</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>New polish time</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be89mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1be8677</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Funny bunny topped w Chrome. Is chrome still a thing? I love it hehe</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulvnjtaj57oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1be7x44</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Jeujed up these $5 nails from AliExpress with a Unicorn Skin taco!</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jdq7moi37oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1be71a1</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>she wins on spring nails</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be71a1</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1be70m5</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>DIY dip powder and ombré</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be70m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1be6rsx</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Finally did the glazed donut nails! 🍩 How did I do?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be6rsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1be6n3e</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Yin-Yanging ☮️</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be6n3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1be6k7e</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>nail alternatives?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1be6k7e/nail_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1be5lg7</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>New press ons!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89tkao1yl6oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1be5iww</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Different nail shapes?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1be5iww/different_nail_shapes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1be59up</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Wanted spring themed nails that would dry quickly while my baby naps, so dotted nails it is!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ibj7t3mj6oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1be4qb2</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Neon Pink Nails for Neon Pink Girls</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0d5f0ldof6oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1be4io5</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Death</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cp9mp8s6e6oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1be4fc7</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Dreamy new set!</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be4fc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1be48ti</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>paint themed 🎨</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be48ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1be45cr</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Should I switch between two nail techs I like</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1be45cr/should_i_switch_between_two_nail_techs_i_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1be2tjw</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>I hate my hands- Help!</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78lxoav826oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1be2xlw</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Inspired by u/Morakva</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07xn077136oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1be350i</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Why don’t I like these?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/woa4uwqe46oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1be3h5n</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>fresh nails🌸🎀</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxk15m1t66oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1be330j</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Normal growth for 2 weeks?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be330j</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1be2th2</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>I tried to do some magical girl nails. Do you like them? ʚ(* ´꒳` *)ɞ💗</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be2th2</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1be0586</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Never had nice nails, compulsive nail biter and skin around biter. What can I do?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be0586</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1bdzs77</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>idk if this is the right place but does anyone have advice to make my nails healthier😭</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdzs77</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1be1rug</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>NEW CLAWS!</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be1rug</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1bdv2h2</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Press on or fake nail recommendations?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdv2h2/press_on_or_fake_nail_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1be1nrj</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Wrap-ons</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti7bv2j0u5oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1be1n22</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Progress</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2jf1slovt5oc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1be10ui</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Is it spring yet?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be10ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1be0y62</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>First ever reddit post. These are some of my favourite sets I have done!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be0y62</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1be0q39</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Latest manicure by my teenage niece</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1wyxejdn5oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1be0c4b</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Not bad for a second try</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be0c4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1be09yb</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Press-on nails. Any tips on how to make them last longer?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be09yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1be09wb</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Imitation/flattery</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be09wb</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1be06ni</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for affordable quality nail salons / artists in the tampa to palm harbor, Florida area? </t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1be06ni/looking_for_affordable_quality_nail_salons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1bdztpb</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Pastel Galaxy</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdztpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1bdzkwe</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>on Wednesdays we wear pink 🩷</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdzkwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1bdz7hd</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Love a good palate cleanser mani 🥰</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdz7hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1bdz0e0</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press On set for my bestie </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/huy9l4ecb5oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1bdy5xf</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>What are these white stuff around my nails?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdy5xf</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1bdy1zm</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Help?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdy1zm/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1bdxu9z</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>They came out so shiny! ✨️</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2djsnqua35oc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1bdx6wt</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Go-to Shade Forever</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z168z5pqy4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1bdx2z0</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Pearly clean galaxy nails</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izgamdnyx4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1bdwu2y</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>new set i did on my natural nails. what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdwu2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1bdwkvy</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Godly vibes ✨</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgogzukeu4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1bdvbz5</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Nails after finals</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdvbz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1bdv004</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Realizing I may have a favorite color 💚</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmk870a7j4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1bduygm</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>First post here</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8x6cjzwvi4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1bdutek</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t xml:space="preserve">St Patrick's nails </t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/T0rtQ4t.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1bduhwq</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>💅</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bduhwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1bdu85p</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>I really suck at taking pictures but my nails turned out great! 🩵</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvjg756jd4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1bdt60r</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdt60r</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1bdt1et</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Pointed nail bed</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tx4nisr44oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1bds52d</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Best at-home gel / shellac polish for a hairstylist?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xu4qj1w0y3oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1bdsm9k</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Ready for spring 🐝</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od2ozv9n14oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1bdsgp3</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>My last few sets. Full coverage gel extensions with gel or dip over top.</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdsgp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1bdsbi0</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Grew my nails out to get gel for the first time in Tokyo!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdsbi0</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1bds2qf</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>first time trying a gray 🩶</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkxogohhx3oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1bdrv21</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1st Attempt and French Tips! </t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbnq6nrtv3oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1bdrmfh</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Dark blue on my natural nails 💙</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnb13wsvt3oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1bdq0bk</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Back to the nub club i go</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdq0bk</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1bdq8eo</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Thoughts on full cover tips/gel X?</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdq8eo/thoughts_on_full_cover_tipsgel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1bdpyex</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set on myself. Acrylic with gel color.  Generic Mickey stickers from Amazon. </t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/detrsnz3f3oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1bdpnom</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pltw2umac3oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1bdpepr</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Self taught &amp; 1st time Acrylic Flowers for Spring nails</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdpepr</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1bdp93j</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Matching March Nails</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdp93j</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1bdp2ez</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very short nails but still looking good. What do you think? </t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugtbm15a63oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1bdoifx</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Preparing for spring 🌱</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olmx9fse03oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1bdnvnf</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Too early to get a fill in?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ode1w1g7t2oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1bdn4q8</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2e6vqaqk2oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1bdm8mb</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Question: Restoring Dried Polish Bottles</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bdm8mb/question_restoring_dried_polish_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1beegs1</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Spring is in the air</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fucbw15nr8oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1bedra1</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Love me a mattefied flaky, especially when it’s giving ~lizard skin~</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ltknoljj8oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1bed5d8</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>I am just too proud of these!</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/td7j5xk4d8oc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1bebyi5</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>DIY magnetic wand?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bebyi5/diy_magnetic_wand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1bearhq</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>St. Patrick's day nails.</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bearhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1beaili</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Clarins 230 &amp; Chanel Sunrise Trip</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beaili</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1beagde</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Mooncat- Pangea x The trouble with immortality</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vh3hsx7mo7oc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1be9tuo</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Can you put gel top coat over regular polish?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1be9tuo/can_you_put_gel_top_coat_over_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1be9sd6</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>1996 Urban Decay Mildew</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be9sd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1be8hhz</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Elopement nail polish recs?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1be8hhz/elopement_nail_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1be8cdw</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Needed a refresh of color</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be8cdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1be8c08</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>La(c)queristas 🤝 cats</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be8c08</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1be78ox</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics Apres Eight</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be78ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1be6jpd</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Emo for Life by Mooncat topped with Electrostatic by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oe8zh8pxs6oc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1be5dm0</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Wasn’t sure if I was going to like or hate this one. The answer is that I LOVE it! Petals for a Narcissist from Mooncat.</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be5dm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1be55lp</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Polishes with INTENSE blue shimmer that aren’t House of Hades?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1be55lp/polishes_with_intense_blue_shimmer_that_arent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1be54cy</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>St Patty’s ☘️🌈🍀💫</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be54cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1be4e9t</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Been getting into nail polish while growing my nails out</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88tlqxkad6oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1be4ah3</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">She's so pretty! </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mr17u7kc6oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1be3z74</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Is it possible to apply gel polish over press on nails before putting the press ons on your actual nails?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1be3z74/is_it_possible_to_apply_gel_polish_over_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1be3im4</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>polish cracks from nail bending? or something else?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be3im4</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1be3ajq</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Dino Sprinkles by Rogue Lacquer</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftjhgz6i56oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1be24j7</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>The closest I get to dressing for St. Patrick's Day</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be24j7</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1be1f96</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Obsessed with Kiara Sky glitters. ✨</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be1f96</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1be0gj7</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>I can't stop looking at my nails 🫣</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be0gj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1be0927</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Green beans...</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgmz70w0k5oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1be03yi</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Shifty multichrome magnetic</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be03yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1bdzrm0</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Thundercloud ⛈️</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdzrm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1bdzm1m</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Am I able to remove these at home?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkh33fdhf5oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1bdpmzg</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Does anyone know what producs have been used to create this look?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdpmzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1bdzlo1</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>day 3 of this mani 🩷</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdzlo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1bdz94u</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Love a good palate cleanser mani 🥰</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdz94u</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1bdz8d4</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>What is your buying/wishlisting process?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bdz8d4/what_is_your_buyingwishlisting_process/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1bdyt6q</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>It's chartreuse, no it's green, wait it's blue, it's just gorgeous 💚🩵</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdyt6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1bdy7o9</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>The 'No Electricity' Mani - 2</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/AEfdyri</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1bdy272</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>How do I stop my nails from breaking &amp; peeling?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h86i73uw45oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1bdy1r8</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Trying to capture the shift</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rf93tl4t45oc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1bdxxjp</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>The 'No Electricity' Mani - 1</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/BUWAYrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1bdxbxq</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>My perfect nude</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdxbxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1bdwh8x</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Fields of Elysium arrived today!!</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwqo7zvpt4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1bdwdyu</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Nail rings - thoughts?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmj63hu2t4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1bdw4m5</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Are Some Brands Incompatible?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g1fnag9r4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1bdvxcg</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Twinning with my sister in law. </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1thvyhhup4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1bdvrfc</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Spring Mix and Match</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdvrfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1bdvqad</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Speckled Monochrome</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdvqad</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1bdvlf4</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Spring nails floral</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdvlf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1bdvimy</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Three weeks of manis</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdvimy</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1bdvg3a</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Realizing I have a favorite color 💚</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ishgda6fm4oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1bdvd63</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>forest drive, my beloved 🌲💚</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdvd63</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1bdpd2m</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>🌱 Polishes Used: ILNP (Shade: Morning Dew) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdpd2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1bdp9bs</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>🪻 Polishes Used: ILNP (Shade: Lilac Bridges) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdp9bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1bdmh3x</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>2nd Gen Urban Decay Brush Replacement?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bdmh3x/2nd_gen_urban_decay_brush_replacement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1bdtyfm</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Reflective polishes are so fun</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdtyfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1bdtdun</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Battle of the Blurples: Polished for Days Goblins and Ghoulies and Similar Polishes</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ueun80o874oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1bdshsp</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Winter vibes!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kk0mll3p04oc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1bdse0y</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>ABCs of polish! O is for Orly!</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owx0q7nxz3oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1bdsbw3</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Aspen has me in a chokehold!</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjoeb9ehz3oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1bdqs8l</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>My St. Pat's Polish</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdqs8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1bdqr2k</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>I stare at my nails constantly when I use this polish</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mxdmv27lm3oc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1bdptcs</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Help! Is there a clear coat that won’t come off with alcohol-based cleaners?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bdptcs/help_is_there_a_clear_coat_that_wont_come_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1bdnpgm</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>EDM - Way Too Far</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdnpgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1bdmnq5</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>I just gave my whole gel polish collection to my mom to use for crafts. Allergies came for me.</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bdmnq5/i_just_gave_my_whole_gel_polish_collection_to_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1beem0p</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>My Halloween set… still my favorite 👻</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beem0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1bee8eg</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Spring is coming 💐</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ry1ngrwwo8oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1bedojz</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>late night set</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bedojz</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1beb4t8</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Just finished painting Fluttershy 💕</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2oqeegxju7oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1bea66l</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>What do you guys think of these?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/roy51r37m7oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1be8vn1</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Pisces birthday beach nails</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1be8vn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1bdz5nc</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Done my birthday-nails</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8afm7dkbc5oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1bdvn3x</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Spring nails floral edition</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdvn3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1bdvem1</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of my design in gray and glitter?
+</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbbfhn35m4oc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1bdtc77</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Did a short sparkly nail set</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdtc77</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1bdqw5r</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Finished one hand of Disney nails</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdqw5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1bdpq1u</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Crystal | Boston Nails 🌼</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bdpq1u</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Mar 15 08:08:04 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_17.xlsx
+++ b/data/2024_03_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C767"/>
+  <dimension ref="A1:C899"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13473,6 +13473,2250 @@
         </is>
       </c>
     </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1bf7wwz</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to you keep your press on? Do you reuse them? </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bf7wwz/how_to_you_keep_your_press_on_do_you_reuse_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1bf7jk7</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>off white chrome nails 🤍</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70tmidm30goc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1bf7j84</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Frog nails?!</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz92eukzzfoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1ber37l</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/100wrytq6coc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1beumza</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Is this a legit brand?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4p93nyonwcoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1bf6i3d</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Don’t let your nails grow out…</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxvk6d9mnfoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1bf6g6b</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>no fixing this?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jtchwjy1nfoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1beolcl</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Wedding nails help! Do you think this design will look good in reality?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beolcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1beliq1</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Nail Tech Ruined My Nails- Help!</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51g5xumg0boc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1bf60m7</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Disastrous nails I did in high school</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/op9j3nxiifoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1bf5u76</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Bf’s sister makes gorgeous press ons</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kh93tplgfoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1bf4t7n</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Finally finished the My little pony set for TikTok 💕 who's your fav?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf4t7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1bf3hcg</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Spring Sparkles!</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qd240r3ueoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1bf368t</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers - Patchwork</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf368t</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1bf30f1</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>She never misses! 🤎</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7bfec71qeoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1bf26f7</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Gel Manicure Peeling</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bf26f7/gel_manicure_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1bf24go</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>My new nails 💓💓</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynekzyfcieoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1bf1zfa</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Spring Green!</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drjjhkk6heoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1bf1so7</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Spring Floral Gel-X Set</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iefmmbmlfeoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1bf1d1v</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>I really want to play guitar but i have to cut one hand short</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bf1d1v/i_really_want_to_play_guitar_but_i_have_to_cut/</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1bf18j2</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>I love black light.</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf18j2</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1bf14pp</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Couldn’t pick a color</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf14pp</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1bf0sno</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>My Press-ons</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3345emb7eoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1bf0fni</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>A perfect pearlescent nude!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5u1v7hbd4eoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1bf09rq</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Best nail glue?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bf09rq/best_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1beztq9</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>One of my biggest pet peeves…</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1beztq9/one_of_my_biggest_pet_peeves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1bez21e</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Lotion gloves</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bez21e/lotion_gloves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1beyonm</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Redid my last set to practice a bit more... Really loving this design! 🩷</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beyonm</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1beyfns</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Is this pinkish color and nail shape flattering?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beyfns</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1beyaei</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>It’s me again asking for you to hype up this color</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmtvou5nndoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1bey4y3</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>rate my nails💚</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bey4y3</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1bexoh9</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Nail grinder</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o73vrf34jdoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1bexi60</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Neon 😚</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnhmn36uhdoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1bex7e2</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>has anyone else had trouble with this remover or is it just me?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6hp50zlfdoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1bex5ve</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>My new set done by me</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bex5ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1bewx91</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Warmer weather vibes (with a falling warrior &lt;/3)</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9ojtefjddoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1bewmhh</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French nails </t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bewmhh/french_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1bewhnk</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Nail color suggestions?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhur1c3cadoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1bev41y</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>How to find your salon?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bev41y/how_to_find_your_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1beuxmi</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Second time DIY Acrylics !</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beuxmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1beuhlk</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>shimmer silver French press ons!</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beuhlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1beu69h</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Barbie Flames 🔥💕</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beu69h</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1bett1s</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails are so much better than they used to be! </t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2e503wlqcoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1bes3ni</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/C4f1JrYMaEx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1berwoq</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite set so far </t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g60kg2xuccoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1ber3g4</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Lollipop pedi set</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ber3g4</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1beqw16</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Lollipop set - part 2</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beqw16</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1beqjoc</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Back to my favorite milky nails 🥛 </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skl10nzt2coc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1beq19c</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Black ombre</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xacd94v4zboc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1beotp7</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Poly gel kawaii junk nails</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/onjhqp3spboc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1beoltg</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Glitterbels builderbels biab! Soya</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r744u4vjoboc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1beo12v</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>I have this client who always wants something simple but still to stand out. I did this design and she said she fell in love. This is a natural square. What do you think?🧚🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beo12v</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1bena50</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>🎀Pink vibes🎀 done by me</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsjlp58deboc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1ben9rz</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>How long should I wait to redo my nails (polygel)?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ben9rz/how_long_should_i_wait_to_redo_my_nails_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1ben7gl</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Haven’t been more satisfied</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvzonrqudboc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1bemq7v</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>💚💛🧡🩷Spring Break Nails💚💛🧡🩷</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bemq7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1belx2y</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtoudbno3boc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1belf6z</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>tips for going through my day with nails?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1belf6z/tips_for_going_through_my_day_with_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1beksyo</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>1,400php</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mau9h8h7uaoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1bekeyo</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Pisces birthday beach set video to see the sparklys ✨</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cilrfexrqaoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1bek6qz</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Are nail salons being affected by the press on nail trend?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bek6qz/are_nail_salons_being_affected_by_the_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1bejw1t</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Something simple for St. Patricks 💖💚</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghk844kklaoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1bejrzc</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my manicure at home after years! </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1lhpa41fkaoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1bej7p1</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Winter wonderland!</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zgmt73ujeaoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1bej7sq</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>The colors reminded me of Skyrim vampires</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bej7sq</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1beil9k</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Got a orange brown! I love the colour. Welcoming spring 🌼</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bou3vjam7aoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1beikvz</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Does such a tool exist?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1beikvz/does_such_a_tool_exist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1bei9j5</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Purple press ons</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bei9j5</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1beh49p</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Minimal and cute - Bara Hoyle</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5x2buxtp9oc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1bf8t2k</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Throwing away nail polish</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bf8t2k/throwing_away_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1bf5vd6</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Anyone else get bothered if you think your mani clashes with your rings?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0oc9866ygfoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1bf5uq4</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Falsies</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lnxhk9rgfoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1bf5u32</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Slainte!</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9oy5sfkgfoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1bf5c2w</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>What should I apply?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bf5c2w/what_should_i_apply/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1bf53xq</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Nail clean up tools tip!</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bf53xq/nail_clean_up_tools_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1bf37e3</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers - Patchwork</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf37e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1bf31dw</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Yet another green mani 🌿</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf31dw</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1bey14t</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Opinion on over filed nails?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/md56m53oldoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1bf2pkc</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jelly skittles manicure 💅 </t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6cs1ikfneoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1bf2nmf</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Blurple comparison + bonus mango jelly</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf2nmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1bf2jey</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">help! </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bf2jey/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1bf1xe4</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>I didn't post these manis for different reasons, until now, what do you think?</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf1xe4</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1bf1ij2</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Disappointed</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf1ij2</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1bf1h24</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>I can’t decide which green to wear. Help!</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6drw66wceoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1bf1ep4</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>unexpectedly love this combination</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf1ep4</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1bf1bwd</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Kiss Me by Cadillacquer</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/18nh8gnobeoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1bf1b1n</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Would you consider this oval?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3dppqohbeoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1bf0p5l</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>how long do i wait until i reapply?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bf0p5l/how_long_do_i_wait_until_i_reapply/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1bf0fn4</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Jelly gradient inspired by the others I’ve seen here 💚🩵</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ml8ep5bd4eoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1bezru1</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>One of my favorites</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bezru1</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1bezisa</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Obsessed with this shade 💖</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bezisa</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1bez253</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Odette + Fairy dust</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dz7gauuitdoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1beyx31</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>My worst break yet 😭</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beyx31</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1beykb1</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Swamp Gloss - Pedro Pascal</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beykb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1bexibw</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>ILNP Brownstone</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9npbckvhdoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1bewe7c</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Tips for shaping?</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngssyz5n9doc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1bew44p</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Expressie - Don’t Glitch Get Better</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bew44p</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1bew2t3</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>ILNP First Light, a disappointment</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bew2t3</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1bew0k1</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Last green-ish mani before I go full shamrock for this weekend ☘️</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bew0k1</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1bevrdz</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>LOOK AT HOW PERFECT THE APPLICATION IS NEAR MY CUTICLES!</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bevrdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1berlkg</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Aquarius 💙✨🦋🌀</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wzq1hg4kacoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1beqz39</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Nailed it! - You Bake Me Happy (May/23 PPU)</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beqz39</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1beqlyx</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Press F to Pay Respects</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2yibvga3coc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1beph1x</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Spring nail art!</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beph1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1beq47k</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>nails still peeling months later</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsl876ppzboc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1bepkad</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Not bad for a drugstore topper</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfjenfzlvboc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1bepfcy</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>mani roundup feb/march</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bepfcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1bepeu0</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>My friday nails 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bepeu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1bep83d</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>New polishes arrived, couldn’t choose which one to try first so I went with both 😌</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bep83d</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1benulh</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Best manicure for a horse girl?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1benulh/best_manicure_for_a_horse_girl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1ben0h1</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Fix: nail started to break too close to nail bed</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ben0h1</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1bemddj</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Zoya Mitzi Frankenpolish</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bemddj</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1bem0ic</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>“Your nails look like they got all dirty with something ” -My dad</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3blhlejg4boc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1belcms</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Boolba</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4s4ex61zyaoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1bel8fg</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>🍀 a lucky skittle 🍀</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bel8fg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1bekixd</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Went for colors in my collection I don't usually go for</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxabqbbmraoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1bej7u1</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Holo + sunlight = a week's worth of distraction</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bej7u1</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1behvof</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Is this dead skin or is it proximal nail fold?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1behvof/is_this_dead_skin_or_is_it_proximal_nail_fold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1beg12n</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Medium/Light Blue Magnetic Nail Polish</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1beg12n/mediumlight_blue_magnetic_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1begogk</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Looking for a regular polish similar to Born Pretty's Jelly Gel Polish in JN14</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1begogk/looking_for_a_regular_polish_similar_to_born/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1beh31f</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Cirque gradient on grandma</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beh31f</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1bf4suq</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Finally finished the My little pony set for TikTok 💕 who's your fav?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf4suq</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1bf1t3b</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Some super long nails</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jg3uxtvnfeoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1bez2x0</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first GelX set, how’d I do? </t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uicur7xotdoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1beyxlp</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Clarissa explains it all</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beyxlp</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1beutzl</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Second time DIY acrylics !</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beutzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1ber5l2</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Lollipop pedi set</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ber5l2</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1beqyg9</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Lollipop set - part 2</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beqyg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1beofkz</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">After I spent 2+ hours on these last night, I just couldn't get the hand to look right, so I decided to put them away. Started over this morning, and I'm so happy with how they came out. </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hu3ep29nboc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1bemn43</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>🧡💚🩷💛Spring Break Vaycay Nails 💚💛🧡🩷</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bemn43</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1bel2xr</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Video to see the sparklies ✨</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9wx65oymwaoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1beju58</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>My take on Jade nails for St Paddy's</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1beju58</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Mar 16 08:07:33 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_17.xlsx
+++ b/data/2024_03_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C899"/>
+  <dimension ref="A1:C1037"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15717,6 +15717,2352 @@
         </is>
       </c>
     </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1bg0q8w</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>My Favorite OPI shade</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg0q8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1bg0m5b</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>HELP. I would like nail glue recommendation for press-ons, vouched by people that have tested and SUCCEEDED past the two week mark.</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bg0m5b/help_i_would_like_nail_glue_recommendation_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1bfzhnn</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Long nails FTW!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfzhnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1bfz9sx</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Fresh set for my birthday week. 💅🏻</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfz9sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1bfz0se</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3pic55wcvmoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1bfybdn</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Just girly pink almonds</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98ona5dknmoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1bfxhe4</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>What is a good natural cuticle oil?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfxhe4/what_is_a_good_natural_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1bfvkrf</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rubber Gel Recommendation </t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfvkrf/rubber_gel_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1bfv04k</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>I'm 37, and for the first time in my life I'm not embarrassed by my nails and skin. 6 weeks of progress, stopped biting.</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfv04k</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1bfwmyd</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>First set after a 6 month “break”🥹</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1k68jha7moc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1bfwip2</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>blue daze 🌀</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjxb0pc66moc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1bfwc6l</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Question about MMA in SnS/Dip nails</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfwc6l/question_about_mma_in_snsdip_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1bfw52q</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Longest they’ve ever been :) Nailtiques Formula 2 is a life saver!</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1brtm0r2moc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1bfw1yl</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>What to do if gel nail falls off</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfw1yl/what_to_do_if_gel_nail_falls_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1bfvix6</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternative to a nail dust collector </t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfvix6/alternative_to_a_nail_dust_collector/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1bfvgh1</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Is hard gel more expensive than dip?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfvgh1/is_hard_gel_more_expensive_than_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1bfuq7p</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>St. Patrick’s here we go……</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ax3ows0qloc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1bfuawy</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ryfglu79mloc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1bftywo</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Simple blush nails 🌸</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bftywo</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1bftnsx</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Loving my nails!!!</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bftnsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1bfswnm</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My manicure, simple but cute. 😊 What do you think? </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvqw5unfaloc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1bfsl8y</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>💚💜</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mojzqydw7loc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1bfsgz4</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Lilac Chrome</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztvc215z6loc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1bfsfs9</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Mushroom nails!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3o6kqap6loc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1bfs8ml</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>a neutral miffy mani 🐰</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfs8ml</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1bfs1bv</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Obsessed with this set. Nail tech cooked</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfs1bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1bfrrdu</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Builder gel isn’t drying</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfrrdu/builder_gel_isnt_drying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1bfrplw</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Feeling green 🌿🍀</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgwycspv0loc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1bfrltz</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Time for a little Easter feeling </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ri59c0310loc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1bfrlbt</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Polish for dark tan skin</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfrlbt/polish_for_dark_tan_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1bfrhpv</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Definitely loving a dark color!</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5patls3zkoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1bfr1pe</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>First go with the French tip stamper.</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngsnfobmvkoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1bfq9ww</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>My wedding nails</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfq9ww</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1bfq8b2</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>At Home Nails</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brbg12t8pkoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1bfpwfn</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Pokémon nails</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfpwfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1bfp21c</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>What can I do for my nails?</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfp21c</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1bfowrb</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Which shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfowrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1bfosch</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Houston, we have Problem! My fav nail tech left the salon, where is he now?</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfosch/houston_we_have_problem_my_fav_nail_tech_left_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1bflfmz</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Manifesting Spriiiing 🪻🌼</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cx1syc0gojoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1bfom2o</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>I love this effect! I can't stop looking at them🩷🥺</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lt72u7hdckoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1bfnmc9</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>They're about to become my whole personnality</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfnmc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1bfn3wg</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>What colour nails would look good with this dress?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5eyjrvx51koc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1bfmykz</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>please help!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfmykz</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1bfmuqg</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Todays client ☘️</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhmluceazjoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1bfmt82</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving the sunset vibes on this set i did yesterday! </t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bql58lnyyjoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1bfmfnw</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Spring nails 💅</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dh28s8f3wjoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1bfm1hl</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>GelX chipping after 3 days :(</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wvus9y2tjoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1bflpy0</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>My best friend did my nails!</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hl9fk4nqjoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1bflo1t</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>A recent diy dip powder mani</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf4pksb8qjoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1bflgb3</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Nervous Newbie.</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bflgb3/nervous_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1bfjwfx</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>My nail tech killed it 👏🏽</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gq2s76htcjoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1bfjvq5</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>first time asking for a design—i’m in love!!</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br4spiaocjoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1bfjllf</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Top coat over builder gel?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfjllf/top_coat_over_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1bfjl0a</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>glue/gel recommendations for press ons</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfjl0a/gluegel_recommendations_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1bfip28</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Just starting out in biab and nail art with zero confidence - opinions welcome / any advice?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfip28</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1bfilcy</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Cirque rosewater jelly</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hanm9v5y2joc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1bfi95k</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Pink with a cute yin yang</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfwcjzeb0joc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1bfi4dg</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>My nail tech is the best 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/um0z08x9zioc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1bfeich</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Does anyone have any idea why this happens?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/64rfneb57ioc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1bf4sjx</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Why does my dip do this?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf4sjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1bf54mn</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Can you share your opinion of my beginner's shopping list? lol</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bf54mn/can_you_share_your_opinion_of_my_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1bfhqqw</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Milky White Nails</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nwhywedwioc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1bfhqpl</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Baby Boomer and abstract nail art with glitter and strass ✨</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfhqpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1bfhdx7</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went for some nudie/ charmy blooming gel claws </t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/defnv4untioc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1bew52j</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Why are my nails so discolored and night white and pretty like other peoples??? Any ideas??</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prlztl5t7doc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1bfgq9q</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Is there a way to put gel x on for just one day?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bfgq9q/is_there_a_way_to_put_gel_x_on_for_just_one_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1bffdxt</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>In case you couldn’t tell, I’m big on gems😍😍</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5h111seaeioc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1bff8zj</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Bright &amp; Vibrant for Spring!</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klllg1o5dioc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1bfdwgo</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>I did these recently</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7gnqrur1ioc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1bfdcw6</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>☘️</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1jvkcmzwhoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1bfcwoy</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Obsession - Magnetic Polish</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afnsdvaqshoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1bfcv2x</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Rubber base gel polish ama</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfcv2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1bfc5sv</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Pink never fails</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf1xgrbflhoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1bfc48l</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>birthday nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfc48l</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1bfbj51</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>First Spring nails of the year. Simple flowers on white base.</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfbj51</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1bfb4yp</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>surprise set from my nailtech</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28tft8wcahoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1bf9y70</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>i do my own nails</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf9y70</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1bf8zwk</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Does this look like a jellybean?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev8gjhgajgoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1bg0cw1</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>First time reverse stamping :)</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg0cw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1bfzpqi</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>My new set 😍</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfzpqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1bfy8xl</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Looks good in daylight too</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfy8xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1bfxqcv</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Replacement for Nailtiques?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bfxqcv/replacement_for_nailtiques/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1bfx333</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ombré nails </t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ovgqhkibmoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1bfv339</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>My Mooncat polishes in their new houses!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74cacqm4tloc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1bfu79y</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which one would you keep and why? </t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9a59jbdlloc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1bftq9b</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Slime/snot green St Patricks nails</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nuh77lc6hloc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1bftenj</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Oops</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mu0slr4meloc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1bfspxo</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Found the perfect nude 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfspxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1bfspmx</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Waiting in line at Costco and took advantage of their lighting. Have a great weekend y’all.</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jus1925w8loc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1bfsbe9</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>a neutral miffy mani 🐰</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfsbe9</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1bfs8ns</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Molten Lava</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uprlfcy35loc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1bfrj8u</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bfrj8u/lurid_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1bfrete</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Shamrock glitter sandwich! 🍀</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rpsrafmfykoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1bfr7cz</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Do I remove both hands knowing I might want to do something green for Sunday?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfr7cz</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1bfqd6m</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Best stain protection base coat?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bfqd6m/best_stain_protection_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1bfq0j9</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Matching with my office wall hehe</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e171hjwknkoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1bfpr5d</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer Rachel Bday Mystery Duoo</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bfpr5d/rogue_lacquer_rachel_bday_mystery_duoo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1bfoy79</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Multichromes 🫶🏾</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfoy79</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1bfojjv</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Lucky Lil' Lizard...</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36wzy828ckoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1bfndlr</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Shein nail polish replacement brush</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfndlr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1bfne7z</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>ILNP Drive In</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfne7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1bfmwrv</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>happy early st. pattys day!!</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfmwrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1bfm37i</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Good weather = good lighting</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9adzywftjoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1bfludq</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>My unconventional green for the weekend. It counts right?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfludq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1bflu1l</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Green Like a dinosaur</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bflu1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1bflmfa</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>OPI Let’s Scrooge: love the colour</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7c3k5ltvpjoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1bfknar</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Tyrannosaurus Hex</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4k96v6dijoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1bfjcle</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Papillon - Super disappointed in Lumen</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfjcle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1bfib26</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>What greens are we rocking for St Patrick’s Day? 🍀</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfib26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1bfi2ds</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Gel nails in red ❤️</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alw1mafuyioc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1bfhig6</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>I love a good thermal flakie</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfhig6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1bfgh1m</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Please help me find out how to make the nailpolish look like the pics below!</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfgh1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1bfgggh</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Just getting into painting my nails and I think I found my favourite colour!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfgggh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1bffk06</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>When I say these were a *struggle*...</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bffk06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1bfel8z</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tip For Leftover QDTCs! </t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bfel8z/tip_for_leftover_qdtcs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1bfd0cj</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying out a new brand </t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jirvmmepthoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1bfcyhq</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Cupcake Polish - Eldhraun</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfcyhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1bfcu5f</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>In love with my new nails!</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfcu5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1bfci1m</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Cirque - Rosewater jelly</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfci1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1bfbsnj</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Feeling ready for Spring Nails</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfbsnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1bfb2ip</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Make it so number one. </t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1b7lzll9hoc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1bfa78i</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>St Patricks day weekend! 🍀</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg4llqvbzgoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1bf9rs8</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Help with thermals and powders?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf9rs8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1bf9b3p</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>La Colors &amp; China Glaze</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bf9b3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1bg00e6</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>First set after a 6 month “break” 🥹</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfa4m5847noc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1bfz24v</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>gel extension tips I did on myself</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfz24v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1bfyaiu</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Getting back into nails after 2 years</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5159prafnmoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1bfvyho</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Gold clovers for St. Patty’s Day ☘️</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfvyho</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1bfrdq4</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>St Patty’s nails by me 🍀🥰</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kb1fp2c5ykoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1bfpd44</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Trying to make my first super easy design 💖💅</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/828723nlikoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1bfp8ac</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Got these nail stickers from shein and they're so pretty 😍</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfp8ac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1bfmge4</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>on me by meeee</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfmge4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1bfk2f3</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>3 hours of work🫠🖤💕</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avt3wc11ejoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1bfjmrd</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Pink Holographic Ombre Nails!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfjmrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1bfhv7f</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>These nails resemble the jade stone 😍</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ohb742bxioc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1bfg5zy</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>I see a lot of us getting our green on ☘️</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugq96948kioc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1bfflvi</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Struggle Shamrocks</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bfflvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1bfdda8</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>☘️</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkz9a2d3xhoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Mar 17 08:07:21 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_17.xlsx
+++ b/data/2024_03_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1037"/>
+  <dimension ref="A1:C1201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18063,6 +18063,2794 @@
         </is>
       </c>
     </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1bgs6kl</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Sunday mani ☺️</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgs6kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1bgr50c</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>a 3 weeks into learning nails!!! my favorite set so far</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dy6sdioeauoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1bgqgot</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Beginner nail tech starting my own business, just did these on myself today!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boda6y5j2uoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1bgqe6d</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>2nd time I’ve ever tried doing my own gel nails!</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/if04h88r1uoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1bgpnkj</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>These press ons look so natural</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6hi9k0ottoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1bgpgxy</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>proud of these!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tl6fse9prtoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1bgpek2</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>It’s like having the night sky at my fingertips</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gc1widaxqtoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1bgp7zd</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Birthday Nails 🦋</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4k2auo4ptoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1bgoyju</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Sacred Heart Manicure</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgoyju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1bghygg</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Polish used in Russian manicure?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bghygg/polish_used_in_russian_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1bghnds</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Gel x nails lifting?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bghnds/gel_x_nails_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1bgoksp</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Press-ons from Etsy!</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3056trxitoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1bgn5uf</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Mini eggs nail inspo</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ynfg66j5toc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1bgogkt</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>i know i knowww, grey and silver nails again</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgogkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1bgnzrr</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Lilac Cat Eye Polish</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgnzrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1bgnyxe</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Hello Kitty pressons vs my unkept nails before (yikes)</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgnyxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1bgnm6i</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>First set on another person (thanks sister!)</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgnm6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1bgn1pp</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>🌼🐰 Easter Nails</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opglosah4toc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1bgmmv9</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Lilac is a good color and I didn’t know it, thanks to my new manicurist</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6weiwkwm0toc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1bgmmhm</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>My new nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6egd775j0toc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1bgm5pg</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Just finished</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22aab1s6wsoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1bglv9h</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Loving this color</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9blgj7tktsoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1bgl13x</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple chrome with Gossip Girl base </t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dn9m02l2msoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1bgkz48</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>St. Paddy’s day nails!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xqrearmjlsoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1bgkso7</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Just got these done today, super happy!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgkso7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1bgkiya</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Finally feeling proud</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgkiya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1bgkeai</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>How did my nails turn out?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgkeai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1bgk9r1</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Gell Stickers</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lozlbjvbfsoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1bgk1id</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Another color changing set 🌙✨</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgk1id</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1bgjmqv</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Painting the end/edge of your nails</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bgjmqv/painting_the_endedge_of_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1bgjk1r</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Love this color in the sun</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9healv599soc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1bgjb09</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>My daughter's spring look🌸</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sad901a67soc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1bgj5o0</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Custom MIFFY press-on nails</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgj5o0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1bgj2un</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>What do you guys think of this manicure?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgj2un</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1bgj1gi</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>been a while since my nails were this long!</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgj1gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1bgikzy</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Is there anything I can do to fix this nail?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgikzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1bgi4wj</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Romantic Rose 🥀</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6d1rxxfxroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1bgi34l</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Can’t get over the fact that my ex said I have monkey hands but here’s my new nails</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgi34l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1bgi122</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Spring nails 🌸</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjcndxegwroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1bghv98</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>My Paddy’s Day Flair ☘️</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0x6bl54vroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1bghtk5</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>New Gel X set for Spring</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bghtk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1bgf4zk</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>What is this white breakage behind the nail after filing? I mean, I'm pretty sure it's bits of nail, but it's hard to remove like it's attached.</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hamlt9zr8roc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1bgdxsu</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Gel vs acrylic for bitten nails??</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bgdxsu/gel_vs_acrylic_for_bitten_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1bgdave</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>What do you guys use to mix polish?</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bgdave/what_do_you_guys_use_to_mix_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1bgglpy</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>St Pattys at home nails :)</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/me58ucgtkroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1bggl8v</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>i did something fun for st. patrick's day</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/554wzfqpkroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1bggfgh</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Textured poisonous dart frog nails</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bggfgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1bgg9yw</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>3rd DIY gel</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx225yv3iroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1bgg1wj</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Baby pink 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgg1wj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1bgg11n</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Tring mate nails.</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyg2nws4groc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1bgfjpn</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Mi nails 💓</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h4x14n6croc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1bgfelr</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love the colour </t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/845mih11broc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1bgfe10</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lilac Cat Eye Nails! </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lhhcg0gwaroc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1bgf57i</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>color match?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rq90art8roc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1bgezjd</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/co3inxmi7roc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1bgelzf</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>New set "Dawn of the sea"</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgelzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1bgdrlq</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ipn0kalxqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1bgcv7h</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Short spring nails!</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63kbrzfdqqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1bgcp1f</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Simple blush nails 🌸</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgcp1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1bgcfjz</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Need help immediately 😫</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hovlh5rwmqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1bgc94r</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Here we go again :(</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0g5z9bilqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1bgc3pc</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to keep less dry skin or cuticle less? I can’t afford manicure often and when I do it myself always cut a lot and is uncomfortable feeling! I don’t like how looks! </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcm33y1bkqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1bgbt1m</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Help please :)</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgbt1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1bgbr28</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gq4gtkgjhqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1bgbevi</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Not loving my new set :(</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezlogkureqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1bgaydc</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving my new press-ons. So shiny and shimmery. </t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjuyrdnabqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1bg98af</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Why is my chrome not smooth?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxonzuboxpoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1bg9ekj</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>First time doing cat eye..</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vncvmqyypoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1bga7e4</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>What do we use to protect surfaces from acetone?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bga7e4/what_do_we_use_to_protect_surfaces_from_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1bga59j</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Biogel vs. Gel X — is there a difference?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bga59j/biogel_vs_gel_x_is_there_a_difference/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1bg9vpy</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">8$ press ons </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2agfc17r2qoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1bg9m23</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Most recent set I did on myself</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg9m23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1bg9i8h</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Air purifier for smell?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bg9i8h/air_purifier_for_smell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1bg9fmx</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzvdttu7zpoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1bg9ae2</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Spring leaves 🌿</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2r89ls4ypoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1bg8p38</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Manifesting spring</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tvqzabetpoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1bg8e0g</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>✨️</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg8e0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1bg8d5b</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg8d5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1bg8csu</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>An emotional day</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg8csu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1bg8a1g</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djho9000qpoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1bg506f</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Why my gel nails always popping off?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcwtxd8zwooc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1bg4iao</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>ridge filler- does it make a difference?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bg4iao/ridge_filler_does_it_make_a_difference/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1bg7vtl</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Short or long nails?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg7vtl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1bg7s67</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Gotta have more green for this weekend!</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0thcvd1zlpoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1bg7ma2</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Feeling cute, might get more later</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg7ma2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1bg766c</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Loving this color combo and the contrast with the zebra!</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yp40d8mqgpoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1bg6o9v</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Trying to decide if my nails are long enough for short coffin</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzzbshnicpoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1bg6kdp</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Boho Spring 🤎</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg6kdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1bg6icd</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Glitter bottoms✨🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/imckcz81bpoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1bg653q</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mum said my nails look horrible </t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pghrqzio7poc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1bg5qca</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>holographic green 💚</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg5qca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1bg5981</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>My bridesmaid nails 🥹</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg5981</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1bg416i</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Dried flowers</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoitdcrnmooc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1bg3dnm</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Pac Man Nails 🕹️ (by charlylousiebeauty)</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg3dnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1bg37jr</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Brand New Set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg37jr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1bg357e</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>I'm always so embaressed😆</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4gdlu07cooc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1bg30su</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Pastel galaxy🩷🪐</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rww4obpnaooc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1bg16se</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Purple coffin nails with bats</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hr2zkw2kmnoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1bgpnq4</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Fastest mani EVER 😀</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bgpnq4/fastest_mani_ever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1bgp28v</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>When doing reverse stamping on a silicone mat to apply over gel polish, is there anything special or different I would need to do for gel vs regular polish?</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bgp28v/when_doing_reverse_stamping_on_a_silicone_mat_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1bgo6pj</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>New HHC nails!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgo6pj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1bgnb4u</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>St. Patrick's Day Nails Bandwagon</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alwn5her6toc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1bgmbza</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s giving midnight under the stars vibes </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1yhcyfuxsoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1bgl8ny</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Wanted something that reminded me of Ectocooler 🤔👻</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgl8ny</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1bgl5m5</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Luckily I'm Frond Of You</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tbpz1s6nsoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1bgk8ny</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>ILNP Maiden Lane - Direct vs. Indirect lighting</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgk8ny</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1bgjyxr</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Sea-ing Is Believing</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51blyofscsoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1bgjhjk</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>St Paddy's manicure</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgjhjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1bgjhie</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>First ILNP Polish!</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgjhie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1bgiuxu</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>I suddenly find myself in possession of a rash of Pigeon themed polishes.</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgiuxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1bgis02</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Favorite Polished For Days perm shades?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bgis02/favorite_polished_for_days_perm_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1bgifzn</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Palate cleanser for interviews 🤍✨</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amfn69myzroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1bgi4pj</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>My Holy Grail</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag553t6exroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1bgi1aj</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Repair done in a bad mood vs repair done in a good mood</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdt70orgwroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1bghqu6</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>3.14 Day might be everyday</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1141153uroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1bgh3dv</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Anyone know why my nail tips are uneven/splotchy?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwtqpauroroc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1bggr2m</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>💚🐸🌱</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mclvgf0mroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1bggmz4</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>They’re not the same! They’re similar</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp96y3f3lroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1bgg3e5</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>🍀</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgg3e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1bgfvxb</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>It Means No Worries 🌹</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgfvxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1bgfne4</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>That moment when</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfkgzrz0droc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1bgf1n3</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>🍀🍀🍀</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgf1n3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1bgexwa</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Sparkly Star Mani</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgexwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1bgewq2</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Luck of the Irish (green)</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/178ykaqv6roc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1bgeavw</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>St. Patrick’s nails</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgeavw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1bgdzu5</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Not a fan of Lights Lacquer, but LOVE their nail Tattoos. Where else can I find these?</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3pk552fzqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1bgdtsl</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Another Canmake Win</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6li6emq2yqoc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1bgdq6u</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>⭐️ Ready for leprechauns!</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgdq6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1bgd3gt</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Blue for today</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fuibtpb8sqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1bgcl8n</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Green for St. Patrick’s Day</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgcl8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1bgckk8</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Essie hard to resist! I've also been using Essie's on a roll cuticle oil lately and I'm obsessed 👀</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o5af8j1oqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1bgcafp</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Clover nails for St. Patrick</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgcafp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1bgc817</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>how do I get rid of the bubbles</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bgc817/how_do_i_get_rid_of_the_bubbles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1bgbqwr</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Spring brights ✨</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm4oo6dihqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1bgbqu0</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>St Patrick's Day mani feat spring decor ☘️🐤</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgbqu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1bgbh91</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Cirque Au Revoir Remover</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgbh91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1bgajog</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>🍐☘️</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4h7h5z28qoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1bg9wjt</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>ILNP - Eclipse</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63atq7hx2qoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1bga7pb</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>st. patrick’s day nails!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hecc1beg5qoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1bg95ex</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Green Pyrex Nails for St. Patty's</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg95ex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1bg8wod</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish Recs for Subtle Star Wars Themed Wedding </t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bg8wod/polish_recs_for_subtle_star_wars_themed_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1bg8rwy</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Festive skittle 🍀🌈</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3o094551upoc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1bg8gkc</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Spring nails are finally here 🌷</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzsn0tggrpoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1bg8eg6</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Mooncat Access Denied</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg8eg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1bg82ll</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>luck o' the irish</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1r5n0kjbopoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1bg7zck</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>I love blue flakies so much 💙</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg7zck</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1bg7xlu</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>St Pats with a little hand drawn art ☘️</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg7xlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1bg7ea5</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Studio Ghibli disappointment</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg7ea5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1bg6v6q</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Feeling lucky 🍀</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nflx1p06epoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1bg6gdi</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Replacement brush question (yes, I did a search, and I still have a question)</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bg6gdi/replacement_brush_question_yes_i_did_a_search_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1bg61wo</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>🪲🪲 on my nails</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gk4y9ot6poc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1bg5vrh</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Matching ♡</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg5vrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1bg58ss</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Please comment what polishes you bought that were NOTHING like their swatch photos</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bg58ss/please_comment_what_polishes_you_bought_that_were/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1bgnftt</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Party nailss</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gym7dbb58toc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1bgnav1</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Junk nails 💅</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgnav1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1bgjofg</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails with a lot of glitter </t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0e1rc1aasoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1bghaiy</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Time to summon some spirits!</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzq3ig2fqroc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1bgc8ye</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>You've an aura about you 🎇</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bgc8ye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1bgbscd</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Famine</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihk3rqauhqoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1bg8hen</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Completed my hand painted ET set</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1radcenrpoc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1bg8eqm</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>did my nails🖤</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/focrfyz1rpoc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1bg6kwn</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Boho Spring</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bg6kwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1bg618i</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Satisfying Top Coat application of candy nails! Looks like a lollipop</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fdv3vhvk6poc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1bg4z2h</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>My new and fav set, I love them so much</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyiwax9owooc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>